<commit_message>
organizing code for Methods
</commit_message>
<xml_diff>
--- a/Supplementary_Data_Tables/Excel_files/Supplementary_Table11_GAP_kinetics.xlsx
+++ b/Supplementary_Data_Tables/Excel_files/Supplementary_Table11_GAP_kinetics.xlsx
@@ -404,7 +404,7 @@
         <color theme="1"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve"> - Michaelis -Menten parameters of GAP-mediated GTP hydrolysis. Standard deviation is based on the three experiment replicates</t>
+      <t xml:space="preserve"> - Michaelis -Menten parameters of GAP-mediated GTP hydrolysis. The two Michaelis-Menten parameters and their ratio (enzymatic efficiency) are determined by an integrated Michaelis-Menten fit for each individual experiment. Standard deviation is based on the 2-9 technical replicates.</t>
     </r>
   </si>
 </sst>
@@ -413,7 +413,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -558,10 +558,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -906,21 +906,21 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="51" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="79" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="72">
       <c r="A2" s="3" t="s">
@@ -949,22 +949,22 @@
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>6.7283295986666598</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>0.77373762170355398</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>5.5711797540000001</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>0.231912446091292</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>1.2056087097861601</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <v>0.147445146529775</v>
       </c>
     </row>
@@ -972,22 +972,22 @@
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>4.3175563070000003</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>1.4650203540772699</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>2.0687996962500002</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>1.1861204065428499</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>2.3770344470876998</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="6">
         <v>1.58363292196695</v>
       </c>
     </row>
@@ -995,22 +995,22 @@
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>5.4207644110000004</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>0.34159678275890998</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>2.2163292623333302</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>0.44831707955148498</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>2.4996102994644298</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="6">
         <v>0.52958651174233695</v>
       </c>
     </row>
@@ -1018,22 +1018,22 @@
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>4.0714149218888798</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>0.96008618611146501</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>1.70717536363333</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>0.67774430601783697</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>2.9725016806228699</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>1.3725557513444699</v>
       </c>
     </row>
@@ -1041,22 +1041,22 @@
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>6.2300556404999998</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>1.68730797044303</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>1.7311843552499999</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <v>0.53252547273708295</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>3.7774084163027699</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="6">
         <v>1.5481534094994001</v>
       </c>
     </row>
@@ -1064,22 +1064,22 @@
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>13.206340279999999</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>3.8808177497313099</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>3.1367771133333302</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>1.13517425819657</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>4.2720771855933801</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="6">
         <v>1.99153759070829</v>
       </c>
     </row>
@@ -1087,22 +1087,22 @@
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>8.9301404101666595</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>0.56065932048141198</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>1.4006595478333299</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>0.21569960076046399</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6">
         <v>6.4820102172585399</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="6">
         <v>1.0779886680827899</v>
       </c>
     </row>
@@ -1110,22 +1110,22 @@
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>5.0261257052000001</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>1.81259901975881</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>0.75141006058000004</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6">
         <v>0.27849869783838499</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>7.1021538831766096</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="6">
         <v>3.6727685223734499</v>
       </c>
     </row>
@@ -1133,22 +1133,22 @@
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="6">
         <v>15.17425879</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>2.2021843978870299</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>2.0404902253333299</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <v>0.17041389207284099</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <v>7.5089905825620198</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="6">
         <v>1.25731533863945</v>
       </c>
     </row>
@@ -1156,22 +1156,22 @@
       <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>3.5243738680000001</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>1.44285265980335E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>0.31835835655</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <v>2.1885807294948299E-2</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <v>11.0951211759562</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="6">
         <v>0.76409453708032604</v>
       </c>
     </row>
@@ -1179,22 +1179,22 @@
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>7.6331000984999999</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <v>1.2955045996847501</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>0.67044983682500003</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="6">
         <v>7.4761394807460094E-2</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="6">
         <v>11.634727725547799</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="6">
         <v>2.36273402392511</v>
       </c>
     </row>
@@ -1202,22 +1202,22 @@
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>5.1863905622499997</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <v>1.2589228252764699</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>0.30032367054999998</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6">
         <v>0.14658774782831899</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <v>19.326487494528202</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="6">
         <v>10.5353561376896</v>
       </c>
     </row>
@@ -1225,22 +1225,22 @@
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>8.9229255174999995</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>1.5195268476795301</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>0.44755020428749998</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <v>0.24291143185598599</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <v>23.896626435450099</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="6">
         <v>13.5935151401584</v>
       </c>
     </row>
@@ -1248,22 +1248,22 @@
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="6">
         <v>8.8293941930000006</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>0.24127677008540399</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>0.30775177266666598</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <v>2.55004662654644E-2</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>28.834850503076702</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="6">
         <v>2.51584729557386</v>
       </c>
     </row>
@@ -1271,22 +1271,22 @@
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>6.3696695794</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>3.6607788790755098</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>0.2389536501</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="6">
         <v>0.10977640107444001</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="6">
         <v>30.301478913710799</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="6">
         <v>22.294889943230199</v>
       </c>
     </row>
@@ -1294,22 +1294,22 @@
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>8.6072102335</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>1.1385352596188401</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <v>0.24875871875</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6">
         <v>6.9735542808130199E-2</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6">
         <v>35.796139827088602</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="6">
         <v>11.0959009880973</v>
       </c>
     </row>
@@ -1317,22 +1317,22 @@
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>4.4628406810000003</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <v>0.99655324610406903</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>0.124153058333333</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6">
         <v>2.13634188962336E-2</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6">
         <v>37.092319066170298</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="6">
         <v>10.456625524808199</v>
       </c>
     </row>
@@ -1340,22 +1340,22 @@
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="6">
         <v>7.8215412782499998</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="6">
         <v>0.64788041872804503</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <v>0.18962363932500001</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="6">
         <v>2.24024177524739E-2</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="6">
         <v>41.9790366042862</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="6">
         <v>6.0570219109501098</v>
       </c>
     </row>
@@ -1363,22 +1363,22 @@
       <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>8.2298123605000004</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="6">
         <v>2.4454621332926898</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>0.19088764252500001</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="6">
         <v>2.8249374592532999E-2</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="6">
         <v>44.717727653356398</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="6">
         <v>14.844474212628301</v>
       </c>
     </row>
@@ -1386,22 +1386,22 @@
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>7.22074108275</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>3.0640722747367901</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>0.13060361815499999</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="6">
         <v>4.6704434801874799E-2</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="6">
         <v>54.210372697817498</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="6">
         <v>30.0830000137165</v>
       </c>
     </row>
@@ -1409,22 +1409,22 @@
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>10.1883856</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <v>0.36806395270787401</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>0.22972962150000001</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="6">
         <v>0.138171879088134</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6">
         <v>54.3990317590643</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="6">
         <v>32.777500232455601</v>
       </c>
     </row>
@@ -1432,22 +1432,22 @@
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>9.1830892960000003</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="6">
         <v>4.4106708142302803E-2</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>0.1500979264</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="6">
         <v>4.8447716754693804E-3</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="6">
         <v>61.224147397712997</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="6">
         <v>1.9979157716314899</v>
       </c>
     </row>
@@ -1455,22 +1455,22 @@
       <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>9.2374493033333298</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="6">
         <v>0.28485117763736101</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>0.1134631272</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="6">
         <v>1.57731654069256E-2</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="6">
         <v>82.300286787546497</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="6">
         <v>11.7191335288909</v>
       </c>
     </row>

</xml_diff>